<commit_message>
Update Match Bank Statement
</commit_message>
<xml_diff>
--- a/public/BankStatement.xlsx
+++ b/public/BankStatement.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>payee</t>
   </si>
@@ -44,22 +44,13 @@
     <t>type</t>
   </si>
   <si>
-    <t>Spend</t>
-  </si>
-  <si>
     <t>ILO</t>
   </si>
   <si>
-    <t>Receive</t>
+    <t>Pendapatan</t>
   </si>
   <si>
-    <t>PLN</t>
-  </si>
-  <si>
-    <t>Biaya Listrik Januari 2020</t>
-  </si>
-  <si>
-    <t>Pendapatan Yayasan Februari 2020</t>
+    <t>Receive</t>
   </si>
 </sst>
 </file>
@@ -435,43 +426,31 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
-        <v>43864</v>
+        <v>43832</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>8</v>
       </c>
       <c r="E2" s="4">
-        <v>150000000</v>
+        <v>250000000</v>
       </c>
       <c r="F2" s="4">
-        <v>150000000</v>
+        <v>250000000</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="2">
-        <v>43871</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="E3" s="4">
-        <v>5000000</v>
-      </c>
-      <c r="F3" s="4">
-        <v>145000000</v>
-      </c>
+      <c r="A3" s="2"/>
+      <c r="B3" s="1"/>
+      <c r="C3" s="1"/>
+      <c r="D3" s="1"/>
+      <c r="E3" s="4"/>
+      <c r="F3" s="4"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="2"/>

</xml_diff>